<commit_message>
Fix email supervisor button - restore email validation in buildSupervisorMailto
</commit_message>
<xml_diff>
--- a/Tables/Employee Information Hub.xlsx
+++ b/Tables/Employee Information Hub.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paula\Projects\uds-asset-management\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0416A582-C469-4815-A6F6-2B2EB9082EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736E5D74-0924-4B12-A007-3653052DA0C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="0" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact Details" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3932" uniqueCount="1727">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3932" uniqueCount="1731">
   <si>
     <t>Last Name</t>
   </si>
@@ -5217,6 +5217,18 @@
   </si>
   <si>
     <t>LAPTOP553</t>
+  </si>
+  <si>
+    <t>masons@udservices.org</t>
+  </si>
+  <si>
+    <t>sarahs@udservices.org</t>
+  </si>
+  <si>
+    <t>shakitaw@udservices.org</t>
+  </si>
+  <si>
+    <t>shannonw@udservices.org</t>
   </si>
 </sst>
 </file>
@@ -5226,10 +5238,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -5252,14 +5272,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -5596,8 +5619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
-      <selection activeCell="E260" sqref="E260"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -17729,8 +17752,8 @@
       <c r="H248" t="s">
         <v>344</v>
       </c>
-      <c r="I248" t="s">
-        <v>33</v>
+      <c r="I248" s="2" t="s">
+        <v>1727</v>
       </c>
       <c r="J248" s="1">
         <v>44564</v>
@@ -18467,8 +18490,8 @@
       <c r="H263" t="s">
         <v>75</v>
       </c>
-      <c r="I263" t="s">
-        <v>33</v>
+      <c r="I263" s="2" t="s">
+        <v>1728</v>
       </c>
       <c r="J263" s="1">
         <v>44417</v>
@@ -19746,8 +19769,8 @@
       <c r="H289" t="s">
         <v>75</v>
       </c>
-      <c r="I289" t="s">
-        <v>33</v>
+      <c r="I289" s="2" t="s">
+        <v>1730</v>
       </c>
       <c r="J289" s="1">
         <v>44452</v>
@@ -19796,8 +19819,8 @@
       <c r="H290" t="s">
         <v>75</v>
       </c>
-      <c r="I290" t="s">
-        <v>33</v>
+      <c r="I290" s="2" t="s">
+        <v>1729</v>
       </c>
       <c r="J290" s="1">
         <v>44431</v>
@@ -20389,9 +20412,15 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I248" r:id="rId1" xr:uid="{8671467D-A347-4343-B2DC-5C85162CAB63}"/>
+    <hyperlink ref="I263" r:id="rId2" xr:uid="{1ACAB52A-F3C8-4B7F-B267-2C79767DFE7A}"/>
+    <hyperlink ref="I290" r:id="rId3" xr:uid="{6F5EC768-F1D0-4517-BCBD-77F0F2E8ECD8}"/>
+    <hyperlink ref="I289" r:id="rId4" xr:uid="{3FA0B97A-31B4-46A8-9D5A-2AD48E58CC9E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>